<commit_message>
add User case 17-18
</commit_message>
<xml_diff>
--- a/report/count.xlsx
+++ b/report/count.xlsx
@@ -12,14 +12,14 @@
     <sheet name="接口覆盖明细表" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">微平台接口开发进度统计汇总!$A$2:$E$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">微平台接口开发进度统计汇总!$A$2:$E$90</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="351">
   <si>
     <t>储值预览</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1408,11 +1408,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>手机开卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/user/bindphone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绑定/修改手机号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>/user/phonecard</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>手机开卡</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1539,7 +1547,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1891,11 +1899,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2025,6 +2057,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2043,14 +2076,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2061,16 +2094,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2404,10 +2445,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2423,12 +2464,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
       <c r="E1" s="25" t="s">
         <v>148</v>
       </c>
@@ -2457,7 +2498,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="67" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2475,7 +2516,7 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="66"/>
+      <c r="A4" s="67"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -2491,7 +2532,7 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="67" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2509,7 +2550,7 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="66"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="2" t="s">
         <v>284</v>
       </c>
@@ -2525,7 +2566,7 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="67" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2543,7 +2584,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="66"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
@@ -2559,7 +2600,7 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="67" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2577,7 +2618,7 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="66"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="2" t="s">
         <v>159</v>
       </c>
@@ -2593,7 +2634,7 @@
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="66"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="11" t="s">
         <v>160</v>
       </c>
@@ -2609,7 +2650,7 @@
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="66"/>
+      <c r="A12" s="67"/>
       <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
@@ -2625,7 +2666,7 @@
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="67" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2643,7 +2684,7 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="66"/>
+      <c r="A14" s="67"/>
       <c r="B14" s="11" t="s">
         <v>282</v>
       </c>
@@ -2659,7 +2700,7 @@
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="66"/>
+      <c r="A15" s="67"/>
       <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
@@ -2675,7 +2716,7 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="66"/>
+      <c r="A16" s="67"/>
       <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
@@ -2691,7 +2732,7 @@
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="66"/>
+      <c r="A17" s="67"/>
       <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
@@ -2707,7 +2748,7 @@
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="66"/>
+      <c r="A18" s="67"/>
       <c r="B18" s="2" t="s">
         <v>37</v>
       </c>
@@ -2723,7 +2764,7 @@
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="66"/>
+      <c r="A19" s="67"/>
       <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
@@ -2739,7 +2780,7 @@
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="66"/>
+      <c r="A20" s="67"/>
       <c r="B20" s="2" t="s">
         <v>41</v>
       </c>
@@ -2755,7 +2796,7 @@
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="67" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -2773,7 +2814,7 @@
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="66"/>
+      <c r="A22" s="67"/>
       <c r="B22" s="11" t="s">
         <v>140</v>
       </c>
@@ -2789,7 +2830,7 @@
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="66"/>
+      <c r="A23" s="67"/>
       <c r="B23" s="2" t="s">
         <v>47</v>
       </c>
@@ -2805,7 +2846,7 @@
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="66"/>
+      <c r="A24" s="67"/>
       <c r="B24" s="59" t="s">
         <v>49</v>
       </c>
@@ -2821,7 +2862,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="66"/>
+      <c r="A25" s="67"/>
       <c r="B25" s="11" t="s">
         <v>51</v>
       </c>
@@ -2837,7 +2878,7 @@
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="66"/>
+      <c r="A26" s="67"/>
       <c r="B26" s="52" t="s">
         <v>300</v>
       </c>
@@ -2853,7 +2894,7 @@
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A27" s="66"/>
+      <c r="A27" s="67"/>
       <c r="B27" s="2" t="s">
         <v>53</v>
       </c>
@@ -2869,7 +2910,7 @@
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A28" s="66"/>
+      <c r="A28" s="67"/>
       <c r="B28" s="2" t="s">
         <v>293</v>
       </c>
@@ -2887,7 +2928,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A29" s="66"/>
+      <c r="A29" s="67"/>
       <c r="B29" s="2" t="s">
         <v>319</v>
       </c>
@@ -2903,7 +2944,7 @@
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A30" s="66"/>
+      <c r="A30" s="67"/>
       <c r="B30" s="2" t="s">
         <v>55</v>
       </c>
@@ -2919,7 +2960,7 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="67" t="s">
         <v>125</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -2937,7 +2978,7 @@
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A32" s="66"/>
+      <c r="A32" s="67"/>
       <c r="B32" s="2" t="s">
         <v>60</v>
       </c>
@@ -2953,7 +2994,7 @@
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A33" s="66"/>
+      <c r="A33" s="67"/>
       <c r="B33" s="52" t="s">
         <v>279</v>
       </c>
@@ -2969,7 +3010,7 @@
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34" s="66"/>
+      <c r="A34" s="67"/>
       <c r="B34" s="52" t="s">
         <v>301</v>
       </c>
@@ -2985,7 +3026,7 @@
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="66"/>
+      <c r="A35" s="67"/>
       <c r="B35" s="2" t="s">
         <v>62</v>
       </c>
@@ -3001,7 +3042,7 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="67" t="s">
         <v>126</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -3019,7 +3060,7 @@
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A37" s="66"/>
+      <c r="A37" s="67"/>
       <c r="B37" s="11" t="s">
         <v>133</v>
       </c>
@@ -3035,7 +3076,7 @@
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A38" s="66"/>
+      <c r="A38" s="67"/>
       <c r="B38" s="2" t="s">
         <v>65</v>
       </c>
@@ -3051,7 +3092,7 @@
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A39" s="66"/>
+      <c r="A39" s="67"/>
       <c r="B39" s="11" t="s">
         <v>141</v>
       </c>
@@ -3067,7 +3108,7 @@
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A40" s="66"/>
+      <c r="A40" s="67"/>
       <c r="B40" s="2" t="s">
         <v>67</v>
       </c>
@@ -3083,7 +3124,7 @@
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A41" s="66"/>
+      <c r="A41" s="67"/>
       <c r="B41" s="2" t="s">
         <v>68</v>
       </c>
@@ -3099,7 +3140,7 @@
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A42" s="66"/>
+      <c r="A42" s="67"/>
       <c r="B42" s="2" t="s">
         <v>70</v>
       </c>
@@ -3115,7 +3156,7 @@
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A43" s="66"/>
+      <c r="A43" s="67"/>
       <c r="B43" s="2" t="s">
         <v>72</v>
       </c>
@@ -3131,7 +3172,7 @@
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="67" t="s">
         <v>127</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -3149,7 +3190,7 @@
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A45" s="66"/>
+      <c r="A45" s="67"/>
       <c r="B45" s="11" t="s">
         <v>135</v>
       </c>
@@ -3165,7 +3206,7 @@
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A46" s="66"/>
+      <c r="A46" s="67"/>
       <c r="B46" s="2" t="s">
         <v>76</v>
       </c>
@@ -3181,7 +3222,7 @@
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A47" s="66"/>
+      <c r="A47" s="67"/>
       <c r="B47" s="11" t="s">
         <v>144</v>
       </c>
@@ -3197,7 +3238,7 @@
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A48" s="66"/>
+      <c r="A48" s="67"/>
       <c r="B48" s="11" t="s">
         <v>135</v>
       </c>
@@ -3213,7 +3254,7 @@
       <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A49" s="66"/>
+      <c r="A49" s="67"/>
       <c r="B49" s="2" t="s">
         <v>78</v>
       </c>
@@ -3229,7 +3270,7 @@
       <c r="F49" s="3"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A50" s="66"/>
+      <c r="A50" s="67"/>
       <c r="B50" s="2" t="s">
         <v>80</v>
       </c>
@@ -3245,7 +3286,7 @@
       <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A51" s="66"/>
+      <c r="A51" s="67"/>
       <c r="B51" s="2" t="s">
         <v>82</v>
       </c>
@@ -3261,7 +3302,7 @@
       <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="67" t="s">
         <v>128</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -3279,7 +3320,7 @@
       <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A53" s="66"/>
+      <c r="A53" s="67"/>
       <c r="B53" s="2" t="s">
         <v>85</v>
       </c>
@@ -3295,7 +3336,7 @@
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A54" s="66"/>
+      <c r="A54" s="67"/>
       <c r="B54" s="2" t="s">
         <v>87</v>
       </c>
@@ -3311,7 +3352,7 @@
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A55" s="66"/>
+      <c r="A55" s="67"/>
       <c r="B55" s="2" t="s">
         <v>89</v>
       </c>
@@ -3327,7 +3368,7 @@
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="67" t="s">
         <v>129</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -3345,7 +3386,7 @@
       <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A57" s="66"/>
+      <c r="A57" s="67"/>
       <c r="B57" s="11" t="s">
         <v>146</v>
       </c>
@@ -3361,7 +3402,7 @@
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A58" s="66"/>
+      <c r="A58" s="67"/>
       <c r="B58" s="2" t="s">
         <v>92</v>
       </c>
@@ -3377,7 +3418,7 @@
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="66"/>
+      <c r="A59" s="67"/>
       <c r="B59" s="59" t="s">
         <v>94</v>
       </c>
@@ -3393,7 +3434,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="66"/>
+      <c r="A60" s="67"/>
       <c r="B60" s="59" t="s">
         <v>200</v>
       </c>
@@ -3409,7 +3450,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A61" s="66"/>
+      <c r="A61" s="67"/>
       <c r="B61" s="2" t="s">
         <v>97</v>
       </c>
@@ -3425,7 +3466,7 @@
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A62" s="66" t="s">
+      <c r="A62" s="77" t="s">
         <v>130</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -3443,7 +3484,7 @@
       <c r="F62" s="3"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A63" s="66"/>
+      <c r="A63" s="78"/>
       <c r="B63" s="11" t="s">
         <v>283</v>
       </c>
@@ -3459,7 +3500,7 @@
       <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A64" s="66"/>
+      <c r="A64" s="78"/>
       <c r="B64" s="2" t="s">
         <v>102</v>
       </c>
@@ -3475,7 +3516,7 @@
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="66"/>
+      <c r="A65" s="78"/>
       <c r="B65" s="59" t="s">
         <v>104</v>
       </c>
@@ -3491,7 +3532,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A66" s="66"/>
+      <c r="A66" s="78"/>
       <c r="B66" s="2" t="s">
         <v>106</v>
       </c>
@@ -3507,7 +3548,7 @@
       <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="66"/>
+      <c r="A67" s="78"/>
       <c r="B67" s="59" t="s">
         <v>108</v>
       </c>
@@ -3523,7 +3564,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A68" s="66"/>
+      <c r="A68" s="78"/>
       <c r="B68" s="2" t="s">
         <v>110</v>
       </c>
@@ -3539,7 +3580,7 @@
       <c r="F68" s="3"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A69" s="66"/>
+      <c r="A69" s="78"/>
       <c r="B69" s="2" t="s">
         <v>112</v>
       </c>
@@ -3555,7 +3596,7 @@
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="66"/>
+      <c r="A70" s="78"/>
       <c r="B70" s="59" t="s">
         <v>114</v>
       </c>
@@ -3571,7 +3612,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="66"/>
+      <c r="A71" s="78"/>
       <c r="B71" s="59" t="s">
         <v>116</v>
       </c>
@@ -3587,7 +3628,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="66"/>
+      <c r="A72" s="78"/>
       <c r="B72" s="59" t="s">
         <v>118</v>
       </c>
@@ -3603,7 +3644,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="66"/>
+      <c r="A73" s="78"/>
       <c r="B73" s="59" t="s">
         <v>119</v>
       </c>
@@ -3619,7 +3660,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A74" s="66"/>
+      <c r="A74" s="78"/>
       <c r="B74" s="2" t="s">
         <v>121</v>
       </c>
@@ -3635,7 +3676,7 @@
       <c r="F74" s="3"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A75" s="66"/>
+      <c r="A75" s="78"/>
       <c r="B75" s="2" t="s">
         <v>321</v>
       </c>
@@ -3651,7 +3692,7 @@
       <c r="F75" s="3"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A76" s="66"/>
+      <c r="A76" s="78"/>
       <c r="B76" s="2" t="s">
         <v>315</v>
       </c>
@@ -3667,7 +3708,7 @@
       <c r="F76" s="3"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A77" s="66"/>
+      <c r="A77" s="78"/>
       <c r="B77" s="2" t="s">
         <v>317</v>
       </c>
@@ -3683,7 +3724,7 @@
       <c r="F77" s="3"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A78" s="66"/>
+      <c r="A78" s="78"/>
       <c r="B78" s="2" t="s">
         <v>323</v>
       </c>
@@ -3699,7 +3740,7 @@
       <c r="F78" s="3"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A79" s="66"/>
+      <c r="A79" s="78"/>
       <c r="B79" s="2" t="s">
         <v>324</v>
       </c>
@@ -3715,7 +3756,7 @@
       <c r="F79" s="3"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A80" s="66"/>
+      <c r="A80" s="78"/>
       <c r="B80" s="2" t="s">
         <v>123</v>
       </c>
@@ -3731,7 +3772,7 @@
       <c r="F80" s="4"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A81" s="54"/>
+      <c r="A81" s="78"/>
       <c r="B81" s="59" t="s">
         <v>327</v>
       </c>
@@ -3747,7 +3788,7 @@
       <c r="F81" s="57"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A82" s="54"/>
+      <c r="A82" s="78"/>
       <c r="B82" s="59" t="s">
         <v>329</v>
       </c>
@@ -3763,7 +3804,7 @@
       <c r="F82" s="57"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A83" s="54"/>
+      <c r="A83" s="78"/>
       <c r="B83" s="59" t="s">
         <v>332</v>
       </c>
@@ -3779,7 +3820,7 @@
       <c r="F83" s="57"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A84" s="54"/>
+      <c r="A84" s="78"/>
       <c r="B84" s="59" t="s">
         <v>333</v>
       </c>
@@ -3795,7 +3836,7 @@
       <c r="F84" s="57"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A85" s="54"/>
+      <c r="A85" s="78"/>
       <c r="B85" s="59" t="s">
         <v>346</v>
       </c>
@@ -3811,7 +3852,7 @@
       <c r="F85" s="57"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A86" s="54"/>
+      <c r="A86" s="78"/>
       <c r="B86" s="59" t="s">
         <v>336</v>
       </c>
@@ -3827,44 +3868,56 @@
       <c r="F86" s="57"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A87" s="54"/>
-      <c r="B87" s="76" t="s">
-        <v>348</v>
-      </c>
-      <c r="C87" s="76" t="s">
+      <c r="A87" s="78"/>
+      <c r="B87" s="61" t="s">
         <v>347</v>
+      </c>
+      <c r="C87" s="61" t="s">
+        <v>350</v>
       </c>
       <c r="D87" s="56"/>
       <c r="E87" s="56"/>
       <c r="F87" s="57"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A88" s="54" t="s">
-        <v>288</v>
-      </c>
-      <c r="B88" s="55" t="str">
-        <f>"共有"&amp; COUNTA(B3:B87)&amp;"个接口"</f>
-        <v>共有85个接口</v>
-      </c>
-      <c r="C88" s="56"/>
+      <c r="A88" s="79"/>
+      <c r="B88" s="61" t="s">
+        <v>349</v>
+      </c>
+      <c r="C88" s="61" t="s">
+        <v>348</v>
+      </c>
       <c r="D88" s="56"/>
       <c r="E88" s="56"/>
       <c r="F88" s="57"/>
     </row>
-    <row r="89" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="16" t="s">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A89" s="54" t="s">
+        <v>288</v>
+      </c>
+      <c r="B89" s="55" t="str">
+        <f>"共有"&amp; COUNTA(B3:B88)&amp;"个接口"</f>
+        <v>共有86个接口</v>
+      </c>
+      <c r="C89" s="56"/>
+      <c r="D89" s="56"/>
+      <c r="E89" s="56"/>
+      <c r="F89" s="57"/>
+    </row>
+    <row r="90" spans="1:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="B89" s="63" t="s">
+      <c r="B90" s="64" t="s">
         <v>151</v>
       </c>
-      <c r="C89" s="64"/>
-      <c r="D89" s="64"/>
-      <c r="E89" s="64"/>
-      <c r="F89" s="65"/>
+      <c r="C90" s="65"/>
+      <c r="D90" s="65"/>
+      <c r="E90" s="65"/>
+      <c r="F90" s="66"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E89">
+  <autoFilter ref="A2:E90">
     <filterColumn colId="4">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -3873,9 +3926,8 @@
   </autoFilter>
   <mergeCells count="14">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="B90:F90"/>
     <mergeCell ref="A56:A61"/>
-    <mergeCell ref="A62:A80"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
@@ -3886,6 +3938,7 @@
     <mergeCell ref="A36:A43"/>
     <mergeCell ref="A44:A51"/>
     <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A62:A88"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3912,13 +3965,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="62" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
       <c r="F1" s="13" t="s">
         <v>148</v>
       </c>
@@ -4290,16 +4343,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="74" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="69"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="76"/>
       <c r="I1" s="40"/>
       <c r="J1" s="39" t="s">
         <v>211</v>
@@ -4345,13 +4398,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="71" t="s">
         <v>274</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="71" t="s">
         <v>227</v>
       </c>
-      <c r="F3" s="70" t="s">
+      <c r="F3" s="71" t="s">
         <v>218</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -4373,9 +4426,9 @@
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
       <c r="G4" s="2" t="s">
         <v>206</v>
       </c>
@@ -4395,9 +4448,9 @@
         <v>3</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
       <c r="G5" s="2" t="s">
         <v>207</v>
       </c>
@@ -4417,9 +4470,9 @@
         <v>4</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="73"/>
       <c r="G6" s="2" t="s">
         <v>208</v>
       </c>
@@ -4439,9 +4492,9 @@
         <v>5</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="70" t="s">
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="71" t="s">
         <v>219</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -4463,9 +4516,9 @@
         <v>6</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
       <c r="G8" s="2" t="s">
         <v>206</v>
       </c>
@@ -4485,9 +4538,9 @@
         <v>7</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
       <c r="G9" s="2" t="s">
         <v>207</v>
       </c>
@@ -4507,9 +4560,9 @@
         <v>8</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="73"/>
       <c r="G10" s="2" t="s">
         <v>225</v>
       </c>
@@ -4529,9 +4582,9 @@
         <v>9</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="70" t="s">
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="71" t="s">
         <v>224</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -4553,9 +4606,9 @@
         <v>10</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
       <c r="G12" s="2" t="s">
         <v>221</v>
       </c>
@@ -4575,9 +4628,9 @@
         <v>11</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
       <c r="G13" s="2" t="s">
         <v>222</v>
       </c>
@@ -4597,9 +4650,9 @@
         <v>12</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
       <c r="G14" s="2" t="s">
         <v>223</v>
       </c>
@@ -4757,13 +4810,13 @@
         <v>18</v>
       </c>
       <c r="C20" s="46"/>
-      <c r="D20" s="73" t="s">
+      <c r="D20" s="68" t="s">
         <v>271</v>
       </c>
-      <c r="E20" s="73" t="s">
+      <c r="E20" s="68" t="s">
         <v>257</v>
       </c>
-      <c r="F20" s="73" t="s">
+      <c r="F20" s="68" t="s">
         <v>269</v>
       </c>
       <c r="G20" s="46" t="s">
@@ -4783,9 +4836,9 @@
         <v>19</v>
       </c>
       <c r="C21" s="46"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
       <c r="G21" s="44" t="s">
         <v>259</v>
       </c>
@@ -4803,9 +4856,9 @@
         <v>20</v>
       </c>
       <c r="C22" s="46"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
       <c r="G22" s="46" t="s">
         <v>260</v>
       </c>
@@ -4823,9 +4876,9 @@
         <v>21</v>
       </c>
       <c r="C23" s="46"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
       <c r="G23" s="46" t="s">
         <v>261</v>
       </c>
@@ -4843,9 +4896,9 @@
         <v>22</v>
       </c>
       <c r="C24" s="46"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="75"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="70"/>
       <c r="G24" s="46" t="s">
         <v>262</v>
       </c>
@@ -4863,9 +4916,9 @@
         <v>23</v>
       </c>
       <c r="C25" s="46"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="73" t="s">
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="68" t="s">
         <v>270</v>
       </c>
       <c r="G25" s="46" t="s">
@@ -4885,9 +4938,9 @@
         <v>24</v>
       </c>
       <c r="C26" s="46"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="48" t="s">
         <v>264</v>
       </c>
@@ -4905,9 +4958,9 @@
         <v>25</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
       <c r="G27" s="2" t="s">
         <v>265</v>
       </c>
@@ -4925,9 +4978,9 @@
         <v>26</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
       <c r="G28" s="2" t="s">
         <v>266</v>
       </c>
@@ -4945,9 +4998,9 @@
         <v>27</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
       <c r="G29" s="2" t="s">
         <v>267</v>
       </c>
@@ -4965,9 +5018,9 @@
         <v>28</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
       <c r="G30" s="2" t="s">
         <v>268</v>
       </c>
@@ -5251,16 +5304,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="E3:E14"/>
     <mergeCell ref="F20:F24"/>
     <mergeCell ref="F25:F30"/>
     <mergeCell ref="E20:E30"/>
     <mergeCell ref="D20:D30"/>
     <mergeCell ref="D3:D14"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="E3:E14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>